<commit_message>
more documentation and reorg
</commit_message>
<xml_diff>
--- a/DOM_Banner/output/dept_banner/Aaron Scott_2023.xlsx
+++ b/DOM_Banner/output/dept_banner/Aaron Scott_2023.xlsx
@@ -1982,7 +1982,7 @@
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W2186113122", "https://openalex.org/W1523310174", "https://openalex.org/W2531913951", "https://openalex.org/W4302381976", "https://openalex.org/W4243634448", "https://openalex.org/W4232219214", "https://openalex.org/W2115543187", "https://openalex.org/W2376557651", "https://openalex.org/W2380323645", "https://openalex.org/W2979752698")</t>
+          <t>c("https://openalex.org/W2186113122", "https://openalex.org/W1523310174", "https://openalex.org/W2531913951", "https://openalex.org/W4302381976", "https://openalex.org/W4243634448", "https://openalex.org/W2115543187", "https://openalex.org/W2376557651", "https://openalex.org/W2380323645", "https://openalex.org/W2979752698", "https://openalex.org/W2391270341")</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>list(au_id = c("https://openalex.org/A5055780915", "https://openalex.org/A5019220974", "https://openalex.org/A5000878326", "https://openalex.org/A5008608447", "https://openalex.org/A5052085802", "https://openalex.org/A5025510544", "https://openalex.org/A5072740048"), au_display_name = c("Don Willis", "Joseph Keawe’aimoku Kaholokula", "Jennifer A. Andersen", "James P. Selig", "Cari A. Bogulski", "Aaron J. Scott", "Pearl A. McElfish"), au_orcid = c("https://orcid.org/0000-0001-9612-489X", "https://orcid.org/0000-0001-5076-6141", 
+          <t>list(au_id = c("https://openalex.org/A5055780915", "https://openalex.org/A5019220974", "https://openalex.org/A5000878326", "https://openalex.org/A5008608447", "https://openalex.org/A5052085802", "https://openalex.org/A5025510544", "https://openalex.org/A5072740048"), au_display_name = c("Don Willis", "Joseph Keawe‘aimoku Kaholokula", "Jennifer A. Andersen", "James P. Selig", "Cari A. Bogulski", "Aaron J. Scott", "Pearl A. McElfish"), au_orcid = c("https://orcid.org/0000-0001-9612-489X", "https://orcid.org/0000-0001-5076-6141", 
 "https://orcid.org/0000-0001-6809-892X", "https://orcid.org/0000-0002-8964-1829", "https://orcid.org/0000-0001-6002-5945", "https://orcid.org/0000-0002-0301-3072", "https://orcid.org/0000-0002-4033-6241"), author_position = c("first", "middle", "middle", "middle", "middle", "middle", "last"), au_affiliation_raw = c("College of Medicine, University of Arkansas for Medical Sciences Northwest, Springdale, USA", "Department of Native Hawaiian Health, John A. Burns School of Medicine, University of Hawai’i at Manoa, Honolulu, USA", 
 "College of Medicine, University of Arkansas for Medical Sciences Northwest, Springdale, USA", "Fay W. Boozman College of Public Health, University of Arkansas for Medical Sciences Northwest, Springdale, USA", "College of Medicine, University of Arkansas for Medical Sciences, Little Rock, USA", "Office of Community Health and Research, University of Arkansas for Medical Sciences Northwest, Springdale, USA", "College of Medicine, University of Arkansas for Medical Sciences Northwest, Springdale, USA"
 ), institution_id = c("https://openalex.org/I79620101", "https://openalex.org/I117965899", "https://openalex.org/I79620101", "https://openalex.org/I79620101", "https://openalex.org/I79620101", "https://openalex.org/I79620101", "https://openalex.org/I79620101"), institution_display_name = c("University of Arkansas for Medical Sciences", "University of Hawaiʻi at Mānoa", "University of Arkansas for Medical Sciences", "University of Arkansas for Medical Sciences", "University of Arkansas for Medical Sciences", 
@@ -4175,7 +4175,7 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W4309211534", "https://openalex.org/W3021434214", "https://openalex.org/W3004259476", "https://openalex.org/W2392730113", "https://openalex.org/W2388808113", "https://openalex.org/W2075214100", "https://openalex.org/W2381416288", "https://openalex.org/W2364051953", "https://openalex.org/W2949011490", "https://openalex.org/W2418638721")</t>
+          <t>c("https://openalex.org/W2472795687", "https://openalex.org/W2471460427", "https://openalex.org/W3121375135", "https://openalex.org/W1499386144", "https://openalex.org/W3140545701", "https://openalex.org/W2990234213", "https://openalex.org/W3042772188", "https://openalex.org/W2139259778", "https://openalex.org/W2374019147", "https://openalex.org/W2063858982")</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr">
@@ -8782,7 +8782,7 @@
       </c>
       <c r="AF47" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W3121695703", "https://openalex.org/W4220656452", "https://openalex.org/W2743577629", "https://openalex.org/W3032149558", "https://openalex.org/W2936810997", "https://openalex.org/W3089461485", "https://openalex.org/W2790732286", "https://openalex.org/W2955998383", "https://openalex.org/W3010513424", "https://openalex.org/W2621190609")</t>
+          <t>c("https://openalex.org/W3035064981", "https://openalex.org/W2769465923", "https://openalex.org/W2897254871", "https://openalex.org/W2112866395", "https://openalex.org/W2137376225", "https://openalex.org/W4238006225", "https://openalex.org/W4389485761", "https://openalex.org/W2092270052", "https://openalex.org/W139966500", "https://openalex.org/W2936650130")</t>
         </is>
       </c>
       <c r="AG47" t="inlineStr">
@@ -8962,7 +8962,7 @@
       </c>
       <c r="AF48" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W2953872710", "https://openalex.org/W2070107750", "https://openalex.org/W2808934676", "https://openalex.org/W1864709827", "https://openalex.org/W1133530171", "https://openalex.org/W1997133872", "https://openalex.org/W2589571971", "https://openalex.org/W2562908937", "https://openalex.org/W2022483081", "https://openalex.org/W2075077394")</t>
+          <t>c("https://openalex.org/W2809146871", "https://openalex.org/W2235788479", "https://openalex.org/W3110357236", "https://openalex.org/W2037039278", "https://openalex.org/W4386281525", "https://openalex.org/W2138294834", "https://openalex.org/W2136984368", "https://openalex.org/W3140349894", "https://openalex.org/W2569965908", "https://openalex.org/W2297296679")</t>
         </is>
       </c>
       <c r="AG48" t="inlineStr">
@@ -9138,7 +9138,7 @@
       </c>
       <c r="AF49" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W3048582358", "https://openalex.org/W1984418710", "https://openalex.org/W2471989939", "https://openalex.org/W4254740740", "https://openalex.org/W1481820868", "https://openalex.org/W4302319510", "https://openalex.org/W2600735778", "https://openalex.org/W2091003848", "https://openalex.org/W2462067466", "https://openalex.org/W2068859133")</t>
+          <t>c("https://openalex.org/W1976837208", "https://openalex.org/W2374639958", "https://openalex.org/W4385644928", "https://openalex.org/W3007979253", "https://openalex.org/W2371775975", "https://openalex.org/W2376040085", "https://openalex.org/W2168671040", "https://openalex.org/W3000564033", "https://openalex.org/W2023453068", "https://openalex.org/W78319162")</t>
         </is>
       </c>
       <c r="AG49" t="inlineStr">

</xml_diff>